<commit_message>
adding stellar parameter from classification.csv
</commit_message>
<xml_diff>
--- a/results/merged_result_MJ.xlsx
+++ b/results/merged_result_MJ.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AT64"/>
+  <dimension ref="A1:AV65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,8 @@
     <col width="12" customWidth="1" min="44" max="44"/>
     <col width="19" customWidth="1" min="45" max="45"/>
     <col width="22" customWidth="1" min="46" max="46"/>
+    <col width="19" customWidth="1" min="47" max="47"/>
+    <col width="13" customWidth="1" min="48" max="48"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -716,6 +718,16 @@
           <t>Density [Solar unit]</t>
         </is>
       </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Distance [pc]</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>V_mag_group</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -874,6 +886,14 @@
       <c r="AT2" t="n">
         <v>2.11927517458269</v>
       </c>
+      <c r="AU2" t="n">
+        <v>19.11360225322881</v>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1029,6 +1049,14 @@
       <c r="AT3" t="n">
         <v>2.052688921124784</v>
       </c>
+      <c r="AU3" t="n">
+        <v>17.86166659875671</v>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1184,6 +1212,14 @@
       <c r="AT4" t="n">
         <v>2.041952602911969</v>
       </c>
+      <c r="AU4" t="n">
+        <v>16.76761069658454</v>
+      </c>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1339,6 +1375,14 @@
       <c r="AT5" t="n">
         <v>2.239104212270826</v>
       </c>
+      <c r="AU5" t="n">
+        <v>19.17020321539005</v>
+      </c>
+      <c r="AV5" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1494,6 +1538,14 @@
       <c r="AT6" t="n">
         <v>1.528241921070437</v>
       </c>
+      <c r="AU6" t="n">
+        <v>14.67227710117747</v>
+      </c>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1652,6 +1704,14 @@
       <c r="AT7" t="n">
         <v>1.621604673108436</v>
       </c>
+      <c r="AU7" t="n">
+        <v>19.62991435281008</v>
+      </c>
+      <c r="AV7" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1807,6 +1867,14 @@
       <c r="AT8" t="n">
         <v>0.8528938169750084</v>
       </c>
+      <c r="AU8" t="n">
+        <v>17.93225480992242</v>
+      </c>
+      <c r="AV8" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1962,6 +2030,14 @@
       <c r="AT9" t="n">
         <v>1.055039360931723</v>
       </c>
+      <c r="AU9" t="n">
+        <v>17.55481503082285</v>
+      </c>
+      <c r="AV9" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2117,6 +2193,14 @@
       <c r="AT10" t="n">
         <v>1.356604055150243</v>
       </c>
+      <c r="AU10" t="n">
+        <v>13.0309238390451</v>
+      </c>
+      <c r="AV10" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2272,6 +2356,14 @@
       <c r="AT11" t="n">
         <v>1.292561167675858</v>
       </c>
+      <c r="AU11" t="n">
+        <v>17.74227354232349</v>
+      </c>
+      <c r="AV11" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2427,6 +2519,14 @@
       <c r="AT12" t="n">
         <v>2.3728520291368</v>
       </c>
+      <c r="AU12" t="n">
+        <v>12.34142491279828</v>
+      </c>
+      <c r="AV12" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2582,6 +2682,14 @@
       <c r="AT13" t="n">
         <v>2.366201403288587</v>
       </c>
+      <c r="AU13" t="n">
+        <v>17.91335395150217</v>
+      </c>
+      <c r="AV13" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2745,6 +2853,14 @@
       <c r="AT14" t="n">
         <v>2.032467946890793</v>
       </c>
+      <c r="AU14" t="n">
+        <v>18.50341299310089</v>
+      </c>
+      <c r="AV14" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2903,6 +3019,14 @@
       <c r="AT15" t="n">
         <v>1.781510507227236</v>
       </c>
+      <c r="AU15" t="n">
+        <v>10.46386619996736</v>
+      </c>
+      <c r="AV15" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3058,6 +3182,14 @@
       <c r="AT16" t="n">
         <v>0.7940434459215121</v>
       </c>
+      <c r="AU16" t="n">
+        <v>14.73911160268253</v>
+      </c>
+      <c r="AV16" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3221,6 +3353,14 @@
       <c r="AT17" t="n">
         <v>1.78211177339737</v>
       </c>
+      <c r="AU17" t="n">
+        <v>18.81162115767776</v>
+      </c>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3376,6 +3516,14 @@
       <c r="AT18" t="n">
         <v>0.906764956917385</v>
       </c>
+      <c r="AU18" t="n">
+        <v>8.534415098502675</v>
+      </c>
+      <c r="AV18" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3534,6 +3682,14 @@
       <c r="AT19" t="n">
         <v>1.457793859010921</v>
       </c>
+      <c r="AU19" t="n">
+        <v>8.791104886960111</v>
+      </c>
+      <c r="AV19" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3692,6 +3848,14 @@
       <c r="AT20" t="n">
         <v>2.745567710296219</v>
       </c>
+      <c r="AU20" t="n">
+        <v>16.39172288343968</v>
+      </c>
+      <c r="AV20" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3842,6 +4006,14 @@
       <c r="AT21" t="n">
         <v>0.8158904314580906</v>
       </c>
+      <c r="AU21" t="n">
+        <v>19.61960010657953</v>
+      </c>
+      <c r="AV21" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3995,6 +4167,14 @@
       <c r="AT22" t="n">
         <v>2.052239288285687</v>
       </c>
+      <c r="AU22" t="n">
+        <v>13.93717968355234</v>
+      </c>
+      <c r="AV22" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -4150,6 +4330,14 @@
       <c r="AT23" t="n">
         <v>1.852212400374402</v>
       </c>
+      <c r="AU23" t="n">
+        <v>18.27507516390551</v>
+      </c>
+      <c r="AV23" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -4313,6 +4501,14 @@
       <c r="AT24" t="n">
         <v>1.769575738741929</v>
       </c>
+      <c r="AU24" t="n">
+        <v>15.71044010482964</v>
+      </c>
+      <c r="AV24" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -4468,6 +4664,14 @@
       <c r="AT25" t="n">
         <v>1.270700200018976</v>
       </c>
+      <c r="AU25" t="n">
+        <v>16.8464974404826</v>
+      </c>
+      <c r="AV25" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -4628,6 +4832,14 @@
       <c r="AT26" t="n">
         <v>1.37647581175124</v>
       </c>
+      <c r="AU26" t="n">
+        <v>12.04471428916949</v>
+      </c>
+      <c r="AV26" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4783,6 +4995,14 @@
       <c r="AT27" t="n">
         <v>2.026252168653316</v>
       </c>
+      <c r="AU27" t="n">
+        <v>18.2083349278885</v>
+      </c>
+      <c r="AV27" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4943,6 +5163,14 @@
       <c r="AT28" t="n">
         <v>0.9403060490214101</v>
       </c>
+      <c r="AU28" t="n">
+        <v>14.136843884035</v>
+      </c>
+      <c r="AV28" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -5098,6 +5326,14 @@
       <c r="AT29" t="n">
         <v>1.226402369197755</v>
       </c>
+      <c r="AU29" t="n">
+        <v>12.57936463354278</v>
+      </c>
+      <c r="AV29" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -5248,6 +5484,14 @@
       <c r="AT30" t="n">
         <v>1.603459718691285</v>
       </c>
+      <c r="AU30" t="n">
+        <v>7.228567098899183</v>
+      </c>
+      <c r="AV30" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -5401,6 +5645,14 @@
       <c r="AT31" t="n">
         <v>1.793063235341547</v>
       </c>
+      <c r="AU31" t="n">
+        <v>19.15340158131814</v>
+      </c>
+      <c r="AV31" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -5553,6 +5805,14 @@
       <c r="AT32" t="n">
         <v>2.241552152343242</v>
       </c>
+      <c r="AU32" t="n">
+        <v>17.56383168799474</v>
+      </c>
+      <c r="AV32" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -5711,6 +5971,14 @@
       <c r="AT33" t="n">
         <v>3.191221396749432</v>
       </c>
+      <c r="AU33" t="n">
+        <v>18.39359418021142</v>
+      </c>
+      <c r="AV33" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -5866,6 +6134,14 @@
       <c r="AT34" t="n">
         <v>1.566652800021061</v>
       </c>
+      <c r="AU34" t="n">
+        <v>17.68739743596811</v>
+      </c>
+      <c r="AV34" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -6021,6 +6297,14 @@
       <c r="AT35" t="n">
         <v>1.953543939316974</v>
       </c>
+      <c r="AU35" t="n">
+        <v>18.67265068138592</v>
+      </c>
+      <c r="AV35" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -6176,6 +6460,14 @@
       <c r="AT36" t="n">
         <v>1.712118408202441</v>
       </c>
+      <c r="AU36" t="n">
+        <v>8.811567976359871</v>
+      </c>
+      <c r="AV36" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -6334,6 +6626,14 @@
       <c r="AT37" t="n">
         <v>2.216291768419251</v>
       </c>
+      <c r="AU37" t="n">
+        <v>3.638438981826665</v>
+      </c>
+      <c r="AV37" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -6484,6 +6784,14 @@
       <c r="AT38" t="n">
         <v>1.114227419076153</v>
       </c>
+      <c r="AU38" t="n">
+        <v>16.95317213092454</v>
+      </c>
+      <c r="AV38" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -6636,6 +6944,14 @@
       <c r="AT39" t="n">
         <v>1.333250845514523</v>
       </c>
+      <c r="AU39" t="n">
+        <v>15.771242532647</v>
+      </c>
+      <c r="AV39" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -6791,6 +7107,14 @@
       <c r="AT40" t="n">
         <v>1.844836198763456</v>
       </c>
+      <c r="AU40" t="n">
+        <v>12.16426728699849</v>
+      </c>
+      <c r="AV40" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -6943,6 +7267,14 @@
       <c r="AT41" t="n">
         <v>1.953362366508123</v>
       </c>
+      <c r="AU41" t="n">
+        <v>7.435229060298576</v>
+      </c>
+      <c r="AV41" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -7098,6 +7430,14 @@
       <c r="AT42" t="n">
         <v>2.324699077934539</v>
       </c>
+      <c r="AU42" t="n">
+        <v>13.59651784149522</v>
+      </c>
+      <c r="AV42" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -7253,6 +7593,14 @@
       <c r="AT43" t="n">
         <v>1.642855324617889</v>
       </c>
+      <c r="AU43" t="n">
+        <v>16.18810659335618</v>
+      </c>
+      <c r="AV43" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -7408,6 +7756,14 @@
       <c r="AT44" t="n">
         <v>1.219684522050477</v>
       </c>
+      <c r="AU44" t="n">
+        <v>15.21037582946627</v>
+      </c>
+      <c r="AV44" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -7563,6 +7919,14 @@
       <c r="AT45" t="n">
         <v>1.75728268109685</v>
       </c>
+      <c r="AU45" t="n">
+        <v>12.93223839703444</v>
+      </c>
+      <c r="AV45" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -7713,6 +8077,14 @@
       <c r="AT46" t="n">
         <v>1.185166893634851</v>
       </c>
+      <c r="AU46" t="n">
+        <v>14.79273794856554</v>
+      </c>
+      <c r="AV46" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -7863,6 +8235,14 @@
       <c r="AT47" t="n">
         <v>2.228367536626836</v>
       </c>
+      <c r="AU47" t="n">
+        <v>19.15843702324353</v>
+      </c>
+      <c r="AV47" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -8021,6 +8401,14 @@
       <c r="AT48" t="n">
         <v>1.450416803044171</v>
       </c>
+      <c r="AU48" t="n">
+        <v>17.30031548819083</v>
+      </c>
+      <c r="AV48" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -8174,6 +8562,14 @@
       <c r="AT49" t="n">
         <v>1.95212998726749</v>
       </c>
+      <c r="AU49" t="n">
+        <v>15.58056293018915</v>
+      </c>
+      <c r="AV49" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -8332,6 +8728,14 @@
       <c r="AT50" t="n">
         <v>2.138539647024254</v>
       </c>
+      <c r="AU50" t="n">
+        <v>13.20790661666426</v>
+      </c>
+      <c r="AV50" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -8487,6 +8891,14 @@
       <c r="AT51" t="n">
         <v>1.717218532617633</v>
       </c>
+      <c r="AU51" t="n">
+        <v>11.44526772917466</v>
+      </c>
+      <c r="AV51" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -8642,6 +9054,14 @@
       <c r="AT52" t="n">
         <v>0.94254112753729</v>
       </c>
+      <c r="AU52" t="n">
+        <v>13.23996519741542</v>
+      </c>
+      <c r="AV52" t="inlineStr">
+        <is>
+          <t>Brightest</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -8800,6 +9220,14 @@
       <c r="AT53" t="n">
         <v>1.747532432148586</v>
       </c>
+      <c r="AU53" t="n">
+        <v>7.601527372616974</v>
+      </c>
+      <c r="AV53" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -8955,6 +9383,14 @@
       <c r="AT54" t="n">
         <v>1.630200033813258</v>
       </c>
+      <c r="AU54" t="n">
+        <v>16.81223174833525</v>
+      </c>
+      <c r="AV54" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -9113,6 +9549,14 @@
       <c r="AT55" t="n">
         <v>1.582829748692533</v>
       </c>
+      <c r="AU55" t="n">
+        <v>14.54849207934481</v>
+      </c>
+      <c r="AV55" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -9268,6 +9712,14 @@
       <c r="AT56" t="n">
         <v>1.15004501453396</v>
       </c>
+      <c r="AU56" t="n">
+        <v>18.34013046861489</v>
+      </c>
+      <c r="AV56" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -9418,6 +9870,14 @@
       <c r="AT57" t="n">
         <v>2.573311979644731</v>
       </c>
+      <c r="AU57" t="n">
+        <v>17.46096412701272</v>
+      </c>
+      <c r="AV57" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -9573,6 +10033,14 @@
       <c r="AT58" t="n">
         <v>1.297074282976997</v>
       </c>
+      <c r="AU58" t="n">
+        <v>10.36054259710993</v>
+      </c>
+      <c r="AV58" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -9731,6 +10199,14 @@
       <c r="AT59" t="n">
         <v>1.865432587008721</v>
       </c>
+      <c r="AU59" t="n">
+        <v>15.28440035086513</v>
+      </c>
+      <c r="AV59" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -9886,6 +10362,14 @@
       <c r="AT60" t="n">
         <v>1.673127109034097</v>
       </c>
+      <c r="AU60" t="n">
+        <v>15.82092734860303</v>
+      </c>
+      <c r="AV60" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -10041,6 +10525,14 @@
       <c r="AT61" t="n">
         <v>1.848206256583958</v>
       </c>
+      <c r="AU61" t="n">
+        <v>14.82647987202467</v>
+      </c>
+      <c r="AV61" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -10196,137 +10688,136 @@
       <c r="AT62" t="n">
         <v>2.895997877367483</v>
       </c>
+      <c r="AU62" t="n">
+        <v>18.72703714229642</v>
+      </c>
+      <c r="AV62" t="inlineStr">
+        <is>
+          <t>Dim</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1827242816201846144</t>
+          <t>3372159045216183552</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>GJ4130</t>
+          <t>GJ233</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="D63" t="n">
         <v>4</v>
       </c>
       <c r="E63" t="n">
-        <v>41.07</v>
+        <v>22750.98</v>
       </c>
       <c r="F63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G63" t="n">
-        <v>7.648</v>
+        <v>0</v>
       </c>
       <c r="H63" t="n">
-        <v>4.5</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="I63" t="n">
-        <v>0.29</v>
+        <v>0.21</v>
       </c>
       <c r="J63" t="n">
-        <v>2.21</v>
+        <v>2.943238</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>K2V</t>
+          <t>K2Ve</t>
         </is>
       </c>
       <c r="L63" s="3" t="n">
-        <v>38928</v>
+        <v>38262</v>
       </c>
       <c r="M63" s="3" t="n">
-        <v>38958</v>
+        <v>38430</v>
       </c>
       <c r="N63" t="n">
-        <v>0.08213552361396304</v>
+        <v>0.459958932238193</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>One known planet, HD 189733b, P 2.2d, 1.13Mj -&gt; HJ. Was observed on only 4 nights, very intensively each night</t>
+          <t>No data on exoplanet archive. 8 obs on 4 nights, huge RV variations!</t>
         </is>
       </c>
       <c r="P63" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q63" t="n">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="S63" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="T63" t="n">
+        <v>4786</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>GJ4130</t>
+          <t>GJ233</t>
         </is>
       </c>
       <c r="V63" t="n">
-        <v>1.827242816201846e+18</v>
+        <v>3.372159045216183e+18</v>
       </c>
       <c r="W63" t="inlineStr">
         <is>
-          <t>1827242816201846144</t>
+          <t>3372159045216183552</t>
         </is>
       </c>
       <c r="X63" t="inlineStr">
         <is>
-          <t>1827242816201846144</t>
+          <t>3372159045216183552</t>
         </is>
       </c>
       <c r="Y63" t="inlineStr">
         <is>
-          <t>1827242816201846144</t>
+          <t>3372159045216183552</t>
         </is>
       </c>
       <c r="Z63" t="n">
-        <v>300.1821218062407</v>
+        <v>96.54210989551521</v>
       </c>
       <c r="AA63" t="n">
-        <v>22.70974110516827</v>
+        <v>18.75620888605506</v>
       </c>
       <c r="AB63" t="n">
-        <v>7.663595725979805</v>
+        <v>6.760678221149445</v>
       </c>
       <c r="AC63" t="n">
-        <v>7.428370952606201</v>
+        <v>6.484982013702393</v>
       </c>
       <c r="AD63" t="n">
-        <v>7.893073081970215</v>
+        <v>6.992666721343994</v>
       </c>
       <c r="AE63" t="n">
-        <v>6.797156810760498</v>
+        <v>5.795860767364502</v>
       </c>
       <c r="AF63" t="n">
-        <v>1.095916271209717</v>
+        <v>1.196805953979492</v>
       </c>
       <c r="AG63" t="n">
-        <v>50.56684941372739</v>
+        <v>68.4141911114458</v>
       </c>
       <c r="AH63" t="n">
-        <v>4897.251</v>
-      </c>
-      <c r="AI63" t="n">
-        <v>0.79787195</v>
+        <v>4602.566867780783</v>
       </c>
       <c r="AJ63" t="n">
-        <v>0.34316152</v>
-      </c>
-      <c r="AK63" t="n">
-        <v>0.8137522</v>
+        <v>0.3698282317554196</v>
       </c>
       <c r="AL63" t="n">
-        <v>0.6007955473381266</v>
+        <v>0.6319064737305783</v>
       </c>
       <c r="AM63" t="n">
-        <v>0.1917407804419631</v>
-      </c>
-      <c r="AN63" t="n">
-        <v>1.484744243946189</v>
+        <v>0.1248168035010945</v>
       </c>
       <c r="AO63" t="inlineStr">
         <is>
@@ -10335,12 +10826,12 @@
       </c>
       <c r="AP63" t="inlineStr">
         <is>
-          <t>HD 189733, HD 189733A</t>
+          <t>HD  45088</t>
         </is>
       </c>
       <c r="AQ63" t="inlineStr">
         <is>
-          <t>GJ 4130</t>
+          <t>GJ 233 A, GJ 233</t>
         </is>
       </c>
       <c r="AS63" t="inlineStr">
@@ -10348,165 +10839,341 @@
           <t>BYDraV*</t>
         </is>
       </c>
-      <c r="AT63" t="n">
-        <v>1.480664521061823</v>
+      <c r="AU63" t="n">
+        <v>14.6168504480454</v>
+      </c>
+      <c r="AV63" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>3330062833797919744</t>
+          <t>1827242816201846144</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>GJ230</t>
+          <t>GJ4130</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="D64" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E64" t="n">
-        <v>5046.08</v>
+        <v>41.07</v>
       </c>
       <c r="F64" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G64" t="n">
+        <v>7.648</v>
       </c>
       <c r="H64" t="n">
-        <v>2.2</v>
+        <v>4.5</v>
       </c>
       <c r="I64" t="n">
-        <v>0.22</v>
+        <v>0.29</v>
       </c>
       <c r="J64" t="n">
-        <v>2.01</v>
+        <v>2.21</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>G5V</t>
+          <t>K2V</t>
         </is>
       </c>
       <c r="L64" s="3" t="n">
-        <v>38340</v>
+        <v>38928</v>
       </c>
       <c r="M64" s="3" t="n">
-        <v>43138</v>
+        <v>38958</v>
       </c>
       <c r="N64" t="n">
-        <v>13.13620807665982</v>
+        <v>0.08213552361396304</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Linear trend? Or seasonal offset? only three RV points in second half, two scattered RV points in between. The activity indices are also offset, which is suspicious. Looking only at season 1 (plot saved), looks like a very nice half of a Keplerian! Wonder why it wasn't continued properly? -&gt; Could be worth fitting out the RV signal, seeing what it looks like -&gt; Fits to 8d, 0.25Mj - HJ? remaining RMS still a bit high</t>
+          <t>One known planet, HD 189733b, P 2.2d, 1.13Mj -&gt; HJ. Was observed on only 4 nights, very intensively each night</t>
         </is>
       </c>
       <c r="P64" t="n">
         <v>9</v>
       </c>
       <c r="Q64" t="n">
-        <v>16</v>
-      </c>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>done</t>
-        </is>
+        <v>2</v>
       </c>
       <c r="S64" t="n">
         <v>1</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
+          <t>GJ4130</t>
+        </is>
+      </c>
+      <c r="V64" t="n">
+        <v>1.827242816201846e+18</v>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>1827242816201846144</t>
+        </is>
+      </c>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>1827242816201846144</t>
+        </is>
+      </c>
+      <c r="Y64" t="inlineStr">
+        <is>
+          <t>1827242816201846144</t>
+        </is>
+      </c>
+      <c r="Z64" t="n">
+        <v>300.1821218062407</v>
+      </c>
+      <c r="AA64" t="n">
+        <v>22.70974110516827</v>
+      </c>
+      <c r="AB64" t="n">
+        <v>7.663595725979805</v>
+      </c>
+      <c r="AC64" t="n">
+        <v>7.428370952606201</v>
+      </c>
+      <c r="AD64" t="n">
+        <v>7.893073081970215</v>
+      </c>
+      <c r="AE64" t="n">
+        <v>6.797156810760498</v>
+      </c>
+      <c r="AF64" t="n">
+        <v>1.095916271209717</v>
+      </c>
+      <c r="AG64" t="n">
+        <v>50.56684941372739</v>
+      </c>
+      <c r="AH64" t="n">
+        <v>4897.251</v>
+      </c>
+      <c r="AI64" t="n">
+        <v>0.79787195</v>
+      </c>
+      <c r="AJ64" t="n">
+        <v>0.34316152</v>
+      </c>
+      <c r="AK64" t="n">
+        <v>0.8137522</v>
+      </c>
+      <c r="AL64" t="n">
+        <v>0.6007955473381266</v>
+      </c>
+      <c r="AM64" t="n">
+        <v>0.1917407804419631</v>
+      </c>
+      <c r="AN64" t="n">
+        <v>1.484744243946189</v>
+      </c>
+      <c r="AO64" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="AP64" t="inlineStr">
+        <is>
+          <t>HD 189733, HD 189733A</t>
+        </is>
+      </c>
+      <c r="AQ64" t="inlineStr">
+        <is>
+          <t>GJ 4130</t>
+        </is>
+      </c>
+      <c r="AS64" t="inlineStr">
+        <is>
+          <t>BYDraV*</t>
+        </is>
+      </c>
+      <c r="AT64" t="n">
+        <v>1.480664521061823</v>
+      </c>
+      <c r="AU64" t="n">
+        <v>19.77580196500298</v>
+      </c>
+      <c r="AV64" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>3330062833797919744</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
           <t>GJ230</t>
         </is>
       </c>
-      <c r="V64" t="n">
+      <c r="C65" t="n">
+        <v>18</v>
+      </c>
+      <c r="D65" t="n">
+        <v>12</v>
+      </c>
+      <c r="E65" t="n">
+        <v>5046.08</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="J65" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>G5V</t>
+        </is>
+      </c>
+      <c r="L65" s="3" t="n">
+        <v>38340</v>
+      </c>
+      <c r="M65" s="3" t="n">
+        <v>43138</v>
+      </c>
+      <c r="N65" t="n">
+        <v>13.13620807665982</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Linear trend? Or seasonal offset? only three RV points in second half, two scattered RV points in between. The activity indices are also offset, which is suspicious. Looking only at season 1 (plot saved), looks like a very nice half of a Keplerian! Wonder why it wasn't continued properly? -&gt; Could be worth fitting out the RV signal, seeing what it looks like -&gt; Fits to 8d, 0.25Mj - HJ? remaining RMS still a bit high</t>
+        </is>
+      </c>
+      <c r="P65" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q65" t="n">
+        <v>16</v>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="S65" t="n">
+        <v>1</v>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>GJ230</t>
+        </is>
+      </c>
+      <c r="V65" t="n">
         <v>3.33006283379792e+18</v>
       </c>
-      <c r="W64" t="inlineStr">
+      <c r="W65" t="inlineStr">
         <is>
           <t>3330062833797919744</t>
         </is>
       </c>
-      <c r="X64" t="inlineStr">
+      <c r="X65" t="inlineStr">
         <is>
           <t>3330062833797919744</t>
         </is>
       </c>
-      <c r="Y64" t="inlineStr">
+      <c r="Y65" t="inlineStr">
         <is>
           <t>3330062833797919744</t>
         </is>
       </c>
-      <c r="Z64" t="n">
+      <c r="Z65" t="n">
         <v>93.30244910592171</v>
       </c>
-      <c r="AA64" t="n">
+      <c r="AA65" t="n">
         <v>10.62581990758492</v>
       </c>
-      <c r="AB64" t="n">
+      <c r="AB65" t="n">
         <v>6.271036148071289</v>
       </c>
-      <c r="AC64" t="n">
+      <c r="AC65" t="n">
         <v>6.271036148071289</v>
       </c>
-      <c r="AD64" t="n">
+      <c r="AD65" t="n">
         <v>6.60129976272583</v>
       </c>
-      <c r="AE64" t="n">
+      <c r="AE65" t="n">
         <v>5.762508869171143</v>
       </c>
-      <c r="AF64" t="n">
+      <c r="AF65" t="n">
         <v>0.8387908935546875</v>
       </c>
-      <c r="AG64" t="n">
+      <c r="AG65" t="n">
         <v>53.76526189706887</v>
       </c>
-      <c r="AH64" t="n">
+      <c r="AH65" t="n">
         <v>5636.9355</v>
       </c>
-      <c r="AI64" t="n">
+      <c r="AI65" t="n">
         <v>0.969942</v>
       </c>
-      <c r="AJ64" t="n">
+      <c r="AJ65" t="n">
         <v>0.7957682</v>
       </c>
-      <c r="AK64" t="n">
+      <c r="AK65" t="n">
         <v>0.93532795</v>
       </c>
-      <c r="AL64" t="n">
+      <c r="AL65" t="n">
         <v>0.8778667036136425</v>
       </c>
-      <c r="AM64" t="n">
+      <c r="AM65" t="n">
         <v>0.1408428551255723</v>
       </c>
-      <c r="AN64" t="n">
+      <c r="AN65" t="n">
         <v>1.453546613752929</v>
       </c>
-      <c r="AO64" t="inlineStr">
+      <c r="AO65" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="AP64" t="inlineStr">
+      <c r="AP65" t="inlineStr">
         <is>
           <t>HD  42807</t>
         </is>
       </c>
-      <c r="AQ64" t="inlineStr">
+      <c r="AQ65" t="inlineStr">
         <is>
           <t>GJ 230</t>
         </is>
       </c>
-      <c r="AS64" t="inlineStr">
+      <c r="AS65" t="inlineStr">
         <is>
           <t>RSCVnV*</t>
         </is>
       </c>
-      <c r="AT64" t="n">
+      <c r="AT65" t="n">
         <v>1.185370263578394</v>
+      </c>
+      <c r="AU65" t="n">
+        <v>18.59937001542844</v>
+      </c>
+      <c r="AV65" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>